<commit_message>
make the catalog works, in an ugly way
</commit_message>
<xml_diff>
--- a/db-misc/schema.xlsx
+++ b/db-misc/schema.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quyendinhthuchoang\Desktop\hack\Projects\code\JavaScript Code\CS 4241\final-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quyendinhthuchoang\Desktop\hack\Projects\code\JavaScript Code\CS 4241\final-project\db-misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -34,21 +34,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>picName</t>
-  </si>
-  <si>
-    <t>accType</t>
-  </si>
-  <si>
-    <t>courseCode</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -89,13 +74,28 @@
   </si>
   <si>
     <t>tomHiddleston</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>picname</t>
+  </si>
+  <si>
+    <t>acctype</t>
+  </si>
+  <si>
+    <t>coursecode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +105,21 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -132,9 +147,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,7 +469,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -471,61 +488,61 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -549,18 +566,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -573,21 +590,22 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.453125" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>